<commit_message>
Adding a new Risk
</commit_message>
<xml_diff>
--- a/project-management/sabolsas-risk.xlsx
+++ b/project-management/sabolsas-risk.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Cliente\project-management\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Risks" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +24,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>SABolsas -  Risk List</t>
   </si>
@@ -237,17 +232,26 @@
   </si>
   <si>
     <t>Tentar quebrar as atividades em pedaços menores, para ser possível cada um dar conta do que foi designado.</t>
+  </si>
+  <si>
+    <t>Problemas Técnicos</t>
+  </si>
+  <si>
+    <t>Atualmente só um integrante possui notebook, em caso de problema, ficamos incapazes de apresentar.</t>
+  </si>
+  <si>
+    <t>Tirar prints das telas que desenvolvemos, para em caso de problemas, ser possível mostrar o andamento do projeto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -601,7 +605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -636,7 +640,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,21 +817,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.42578125"/>
     <col min="2" max="2" width="10.140625"/>
@@ -843,7 +847,7 @@
     <col min="27" max="1025" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +877,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="65.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -921,7 +925,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="25.5" customHeight="1">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -970,7 +974,7 @@
       <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="25.5" customHeight="1">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -1019,7 +1023,7 @@
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
     </row>
-    <row r="5" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="25.5" customHeight="1">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -1068,7 +1072,7 @@
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="38.25" customHeight="1">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1117,7 +1121,7 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="25.5" customHeight="1">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1166,7 +1170,7 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="A8" s="6">
         <v>9</v>
       </c>
@@ -1215,7 +1219,7 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="62.25" customHeight="1">
       <c r="A9" s="6">
         <v>10</v>
       </c>
@@ -1264,7 +1268,7 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
     </row>
-    <row r="10" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="57" customHeight="1">
       <c r="A10" s="6">
         <v>11</v>
       </c>
@@ -1313,7 +1317,7 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
     </row>
-    <row r="11" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="27" customHeight="1">
       <c r="A11" s="6">
         <v>12</v>
       </c>
@@ -1362,7 +1366,7 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
     </row>
-    <row r="12" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="59.25" customHeight="1">
       <c r="A12" s="6">
         <v>13</v>
       </c>
@@ -1411,7 +1415,7 @@
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
     </row>
-    <row r="13" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="50.25" customHeight="1">
       <c r="A13" s="6">
         <v>14</v>
       </c>
@@ -1460,22 +1464,38 @@
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
     </row>
-    <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="43.5" customHeight="1">
       <c r="A14" s="6">
         <v>15</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="8"/>
+      <c r="B14" s="7">
+        <v>42934</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="6">
+        <v>5</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
       <c r="H14" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -1493,7 +1513,7 @@
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="12.75" customHeight="1">
       <c r="A15" s="6">
         <v>16</v>
       </c>
@@ -1526,7 +1546,7 @@
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="12.75" customHeight="1">
       <c r="A16" s="6">
         <v>17</v>
       </c>
@@ -1559,7 +1579,7 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
     </row>
-    <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="12.75" customHeight="1">
       <c r="A17" s="6">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Updating PM and Risks
</commit_message>
<xml_diff>
--- a/project-management/sabolsas-risk.xlsx
+++ b/project-management/sabolsas-risk.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Risks" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -817,7 +817,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -828,7 +828,7 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1043,11 +1043,11 @@
         <v>5</v>
       </c>
       <c r="G5" s="8">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>17</v>
@@ -1288,11 +1288,11 @@
         <v>5</v>
       </c>
       <c r="G10" s="13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>17</v>
@@ -1337,11 +1337,11 @@
         <v>5</v>
       </c>
       <c r="G11" s="8">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>17</v>
@@ -1386,11 +1386,11 @@
         <v>4</v>
       </c>
       <c r="G12" s="8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>17</v>
@@ -1435,11 +1435,11 @@
         <v>5</v>
       </c>
       <c r="G13" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Adding new Iteration and Risks
</commit_message>
<xml_diff>
--- a/project-management/sabolsas-risk.xlsx
+++ b/project-management/sabolsas-risk.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>SABolsas -  Risk List</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Tirar prints das telas que desenvolvemos, para em caso de problemas, ser possível mostrar o andamento do projeto.</t>
+  </si>
+  <si>
+    <t>Migração para o novo Layout</t>
+  </si>
+  <si>
+    <t>Nosso sistema terá o layout migrado para o padrão da outra equipe.</t>
+  </si>
+  <si>
+    <t>Pelo fato de cada equipe estar usando frameworks diferentes, é certo que um não cobrirá todas as possibilidades do outro, por isso, vamos sugerir caso necessário, utilizar os dois frameworks mantendo um padrão no Layout.</t>
   </si>
 </sst>
 </file>
@@ -817,7 +826,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -828,7 +837,7 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1513,22 +1522,36 @@
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1">
+    <row r="15" spans="1:26" ht="63.75" customHeight="1">
       <c r="A15" s="6">
         <v>16</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8"/>
+      <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="6">
+        <v>3</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.5</v>
+      </c>
       <c r="H15" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>

</xml_diff>